<commit_message>
Ajuste no script para consultar a cidade de acordo com a entrada do usuário
</commit_message>
<xml_diff>
--- a/historico_temperatura.xlsx
+++ b/historico_temperatura.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,87 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>16/02/2025 21:42:34</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>58%</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Média Umidade no ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>16/02/2025 21:46:05</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>58%</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Média Umidade no ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>16/02/2025 21:46:57</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Taboão da Serra</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>60%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Alerta Amarelo, Média Umidade no ar</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>